<commit_message>
mejora de comprobacion de overwrite + rename de archivos
</commit_message>
<xml_diff>
--- a/playlist_tracks.xlsx
+++ b/playlist_tracks.xlsx
@@ -1549,7 +1549,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=9j4f67o_5iw</t>
+          <t>https://www.youtube.com/watch?v=sfHG9Vg-ELE</t>
         </is>
       </c>
     </row>
@@ -2361,27 +2361,27 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Fin de Semana</t>
+          <t>Adicto</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Anonimus, Julio H, Mr. Saik</t>
+          <t>Carlitos Rossy, Dalex</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Fin de Semana</t>
+          <t>Sad Valentín</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2024-07-05</t>
+          <t>2023-05-25</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=VZkXHpbQedo</t>
+          <t>https://www.youtube.com/watch?v=URvNDDbLIZ8</t>
         </is>
       </c>
     </row>
@@ -2925,7 +2925,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=YR1t_MUN8I4</t>
+          <t>https://www.youtube.com/watch?v=EY-nAOFpenI</t>
         </is>
       </c>
     </row>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=DPx2YgYTA-8</t>
+          <t>https://www.youtube.com/watch?v=6HgF6T02ZBY</t>
         </is>
       </c>
     </row>
@@ -4077,7 +4077,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=TiM_TFpT_DE</t>
+          <t>https://www.youtube.com/watch?v=D6Ju9CyOB-I</t>
         </is>
       </c>
     </row>
@@ -4941,7 +4941,7 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=US3Rq8cQt9g</t>
+          <t>https://www.youtube.com/watch?v=WENoupAz5C0</t>
         </is>
       </c>
     </row>
@@ -5561,27 +5561,27 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Maquillaje</t>
+          <t>SUERTE</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Renn, Yexel</t>
+          <t>Renn</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>Maquillaje</t>
+          <t>SUERTE</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>2024-01-10</t>
+          <t>2023-03-23</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=I9_21ocFM9o</t>
+          <t>https://www.youtube.com/watch?v=Kn3OJ2njI6Y</t>
         </is>
       </c>
     </row>
@@ -5593,27 +5593,27 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>SUERTE</t>
+          <t>PAGANI</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Renn</t>
+          <t>BLANKO</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>SUERTE</t>
+          <t>PAGANI</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>2023-03-23</t>
+          <t>2024-05-03</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Kn3OJ2njI6Y</t>
+          <t>https://www.youtube.com/watch?v=mtDMUPmmsnk</t>
         </is>
       </c>
     </row>
@@ -5625,27 +5625,27 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>PAGANI</t>
+          <t>Alto Troyanaje</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>BLANKO</t>
+          <t>Waldokinc El Troyano</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>PAGANI</t>
+          <t>Nivel 2</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>2024-05-03</t>
+          <t>2013-04-30</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=mtDMUPmmsnk</t>
+          <t>https://www.youtube.com/watch?v=bjaa8L37xbM</t>
         </is>
       </c>
     </row>
@@ -5657,27 +5657,27 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Alto Troyanaje</t>
+          <t>Ve y Diles</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Waldokinc El Troyano</t>
+          <t>Alex Ponce, Sebastian Llosa</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Nivel 2</t>
+          <t>Ve y Diles</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>2013-04-30</t>
+          <t>2024-05-09</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=bjaa8L37xbM</t>
+          <t>https://www.youtube.com/watch?v=Qhw83uv0RUs</t>
         </is>
       </c>
     </row>
@@ -5689,27 +5689,27 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Ve y Diles</t>
+          <t>VIP</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Alex Ponce, Sebastian Llosa</t>
+          <t>Milo Mae</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>Ve y Diles</t>
+          <t>LO TOP, LO EXCLUSIVE</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>2024-05-09</t>
+          <t>2024-02-16</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Qhw83uv0RUs</t>
+          <t>https://www.youtube.com/watch?v=_vnr3ZtQRBg</t>
         </is>
       </c>
     </row>
@@ -5721,27 +5721,27 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>VIP</t>
+          <t>Una y otra vez</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Milo Mae</t>
+          <t>Vincez, Milo Mae, Deep Nao</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>LO TOP, LO EXCLUSIVE</t>
+          <t>Una y otra vez</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>2024-02-16</t>
+          <t>2024-05-03</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=_vnr3ZtQRBg</t>
+          <t>https://www.youtube.com/watch?v=bQWS4WGiLhA</t>
         </is>
       </c>
     </row>
@@ -5753,27 +5753,27 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Una y otra vez</t>
+          <t>PLAYER</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Vincez, Milo Mae, Deep Nao</t>
+          <t>Carlos Corté$</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Una y otra vez</t>
+          <t>PLAYER</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>2024-05-03</t>
+          <t>2023-09-01</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=bQWS4WGiLhA</t>
+          <t>https://www.youtube.com/watch?v=X3qfOg9X7hQ</t>
         </is>
       </c>
     </row>
@@ -5785,7 +5785,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>PLAYER</t>
+          <t>CONTIGO</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -5795,17 +5795,17 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>PLAYER</t>
+          <t>PACK VERANO 002</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>2023-09-01</t>
+          <t>2022-08-26</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=X3qfOg9X7hQ</t>
+          <t>https://www.youtube.com/watch?v=TUspIUD8t_s</t>
         </is>
       </c>
     </row>
@@ -5817,27 +5817,27 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>CONTIGO</t>
+          <t>SEXATON</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Carlos Corté$</t>
+          <t>Milo Mae, Carlos Corté$, Kenny Die, Vyse</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>PACK VERANO 002</t>
+          <t>LO TOP, LO EXCLUSIVE</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>2022-08-26</t>
+          <t>2024-02-16</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=TUspIUD8t_s</t>
+          <t>https://www.youtube.com/watch?v=yr_vgcdAyKk</t>
         </is>
       </c>
     </row>
@@ -5849,27 +5849,27 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>SEXATON</t>
+          <t>Tu para Mi</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Milo Mae, Carlos Corté$, Kenny Die, Vyse</t>
+          <t>Kenny Die</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>LO TOP, LO EXCLUSIVE</t>
+          <t>Tu para Mi</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>2024-02-16</t>
+          <t>2022-06-16</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=yr_vgcdAyKk</t>
+          <t>https://www.youtube.com/watch?v=P59nEZ-8mDo</t>
         </is>
       </c>
     </row>
@@ -5881,27 +5881,27 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Tu para Mi</t>
+          <t>Titerito</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Kenny Die</t>
+          <t>Ecby, Milo Mae, Strauss</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Tu para Mi</t>
+          <t>Titerito</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>2022-06-16</t>
+          <t>2024-06-13</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=P59nEZ-8mDo</t>
+          <t>https://www.youtube.com/watch?v=I6THGFRfBDg</t>
         </is>
       </c>
     </row>
@@ -5913,27 +5913,27 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Titerito</t>
+          <t>Casa Blanca</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Ecby, Milo Mae, Strauss</t>
+          <t>Mersa</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>Titerito</t>
+          <t>Casa Blanca</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>2024-06-13</t>
+          <t>2024-02-13</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=I6THGFRfBDg</t>
+          <t>https://www.youtube.com/watch?v=4eBG5zOrJW4</t>
         </is>
       </c>
     </row>
@@ -5945,27 +5945,27 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Casa Blanca</t>
+          <t>Lunares</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Mersa</t>
+          <t>Mersa, Mr Reo, Kiff</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Casa Blanca</t>
+          <t>Lunares</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>2024-02-13</t>
+          <t>2024-05-31</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=4eBG5zOrJW4</t>
+          <t>https://www.youtube.com/watch?v=ddbluhWj-EA</t>
         </is>
       </c>
     </row>
@@ -5977,27 +5977,27 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Lunares</t>
+          <t>Como tu no hay otra</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Mersa, Mr Reo, Kiff</t>
+          <t>Dayan</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Lunares</t>
+          <t>Buena Suerte y Adios</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>2024-05-31</t>
+          <t>2024-03-29</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ddbluhWj-EA</t>
+          <t>https://www.youtube.com/watch?v=WeOPkKxP_E0</t>
         </is>
       </c>
     </row>
@@ -6009,27 +6009,27 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Como tu no hay otra</t>
+          <t>Noche De Amanecia</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Dayan</t>
+          <t>Renn</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>Buena Suerte y Adios</t>
+          <t>Noche De Amanecia</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-07-19</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=WeOPkKxP_E0</t>
+          <t>https://www.youtube.com/watch?v=oUXI0Gf0x_w</t>
         </is>
       </c>
     </row>

</xml_diff>